<commit_message>
update velocity chart sprint 1
</commit_message>
<xml_diff>
--- a/Reviews/Sprint_Velocity_Chart.xlsx
+++ b/Reviews/Sprint_Velocity_Chart.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\phili\Desktop\github_projekte\SYP_GRUPPE_3_2024\Reviews\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECEE1D46-8478-41F6-B92C-B4E643CE849D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{952583F9-9D32-4E43-B180-A74FDFE168C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3060" yWindow="1530" windowWidth="21600" windowHeight="11385" xr2:uid="{08BCE8FC-179B-459C-9B7D-265214947282}"/>
+    <workbookView xWindow="930" yWindow="1590" windowWidth="21600" windowHeight="11385" xr2:uid="{08BCE8FC-179B-459C-9B7D-265214947282}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -203,7 +203,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>10</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1398,8 +1398,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2F7B7D6-30CA-4B00-92E5-61B05DCAC22F}">
   <dimension ref="B3:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q15" sqref="Q15:R15"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1414,7 +1414,7 @@
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C4">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
pp sprint 4 und charts
</commit_message>
<xml_diff>
--- a/Reviews/Sprint_Velocity_Chart.xlsx
+++ b/Reviews/Sprint_Velocity_Chart.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\phili\Desktop\github_projekte\SYP_GRUPPE_3_2024\Reviews\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB120B40-AE51-4BFD-8D38-15D16B7D4ADD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A97F66F-F5F9-449D-9C17-2E7BEC282CD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{08BCE8FC-179B-459C-9B7D-265214947282}"/>
   </bookViews>
@@ -208,10 +208,10 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>Tabelle1!$D$5:$D$7</c:f>
+              <c:f>Tabelle1!$D$5:$D$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>7</c:v>
                 </c:pt>
@@ -220,6 +220,9 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>13</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1415,7 +1418,7 @@
   <dimension ref="B4:P16"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1434,7 +1437,7 @@
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B5">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D5">
         <v>7</v>
@@ -1450,13 +1453,18 @@
         <v>31</v>
       </c>
     </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D8">
+        <v>13</v>
+      </c>
+    </row>
     <row r="16" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>2</v>
       </c>
       <c r="C16">
-        <f>(D5+D6+D7)/B5</f>
-        <v>19</v>
+        <f>(D5+D6+D7+D8)/B5</f>
+        <v>17.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>